<commit_message>
Update test inputs using 10-13-22 PEARS schema
</commit_message>
<xml_diff>
--- a/tests/expected_outputs/Quarterly Coalition Survey Entry Q4.xlsx
+++ b/tests/expected_outputs/Quarterly Coalition Survey Entry Q4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="172">
   <si>
     <t>Module</t>
   </si>
@@ -191,12 +191,39 @@
     <t>9121</t>
   </si>
   <si>
+    <t>9131</t>
+  </si>
+  <si>
+    <t>9133</t>
+  </si>
+  <si>
+    <t>9173</t>
+  </si>
+  <si>
+    <t>9243</t>
+  </si>
+  <si>
     <t>9322</t>
   </si>
   <si>
+    <t>9349</t>
+  </si>
+  <si>
+    <t>9350</t>
+  </si>
+  <si>
     <t>9581</t>
   </si>
   <si>
+    <t>9627</t>
+  </si>
+  <si>
+    <t>9724</t>
+  </si>
+  <si>
+    <t>9728</t>
+  </si>
+  <si>
     <t>Coalition Data 7621 Coalition Name</t>
   </si>
   <si>
@@ -317,70 +344,118 @@
     <t>Coalition Data 9121 Coalition Name</t>
   </si>
   <si>
+    <t>Coalition Data 9131 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9133 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9173 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9243 Coalition Name</t>
+  </si>
+  <si>
     <t>Coalition Data 9322 Coalition Name</t>
   </si>
   <si>
+    <t>Coalition Data 9349 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9350 Coalition Name</t>
+  </si>
+  <si>
     <t>Coalition Data 9581 Coalition Name</t>
   </si>
   <si>
-    <t>Chad.Smith@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Monique.James@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Frank.Lewis@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Thomas.Cook@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Richard.Robertson@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Terry.Mcdonald@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Jordan.Williams@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Jeffrey.Hanson@fake_domain.com</t>
-  </si>
-  <si>
-    <t>David.Gomez@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Cody.Miller@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Kathleen.Munoz@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Dr.Calvin.Baker@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Ms.Kelly.Mccann.MD@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Carmen.Matthews@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Pamela.Ramsey@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Cassandra.Ford@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Michelle.Mcintosh@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Michelle.Robinson@fake_domain.com</t>
-  </si>
-  <si>
-    <t>William.Hurst@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Amber.Wilson@fake_domain.com</t>
+    <t>Coalition Data 9627 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9724 Coalition Name</t>
+  </si>
+  <si>
+    <t>Coalition Data 9728 Coalition Name</t>
+  </si>
+  <si>
+    <t>Jean.Fitzgerald@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Laura.Garrett@fake_domain.com</t>
+  </si>
+  <si>
+    <t>David.Kane@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Mary.Baker@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Stephanie.Patterson@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Pamela.Rubio@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Wayne.Johnston@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Angela.Shannon@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Joseph.Miller@fake_domain.com</t>
+  </si>
+  <si>
+    <t>James.Page@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Jamie.Hunter@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Matthew.Murphy@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Sandra.Alvarez@fake_domain.com</t>
+  </si>
+  <si>
+    <t>William.Porter@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Dawn.Barker@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Alexander.Smith@fake_domain.com</t>
+  </si>
+  <si>
+    <t>James.Phillips@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Chelsea.Harper@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Kimberly.Dunn@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Edward.Joseph@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Francisco.Brock@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Angela.Thompson@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Dr.David.Dunn@fake_domain.com</t>
+  </si>
+  <si>
+    <t>James.Long@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Amber.Smith@fake_domain.com</t>
+  </si>
+  <si>
+    <t>April.Bowman@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Joshua.James@fake_domain.com</t>
   </si>
   <si>
     <t>22</t>
@@ -428,7 +503,19 @@
     <t>8</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>24</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t>Collaboration</t>
@@ -841,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -869,7 +956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -877,7 +964,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="66.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -912,19 +999,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -935,19 +1022,19 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -958,19 +1045,19 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -981,19 +1068,19 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -1004,19 +1091,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -1027,19 +1114,19 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -1050,19 +1137,19 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -1073,19 +1160,19 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -1096,19 +1183,19 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F10" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -1119,19 +1206,19 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -1142,19 +1229,19 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F12" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -1165,19 +1252,19 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -1188,19 +1275,19 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1211,19 +1298,19 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1234,19 +1321,19 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1257,19 +1344,19 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F17" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1280,19 +1367,19 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -1303,19 +1390,19 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F19" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1326,19 +1413,19 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F20" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1349,19 +1436,19 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F21" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -1372,19 +1459,19 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -1395,19 +1482,19 @@
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F23" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -1418,19 +1505,19 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
@@ -1441,19 +1528,19 @@
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
@@ -1464,19 +1551,19 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
@@ -1487,19 +1574,19 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F27" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -1510,19 +1597,19 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F28" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
@@ -1533,19 +1620,19 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F29" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G29" t="s">
         <v>8</v>
@@ -1556,19 +1643,19 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G30" t="s">
         <v>8</v>
@@ -1579,19 +1666,19 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G31" t="s">
         <v>8</v>
@@ -1602,19 +1689,19 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F32" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
@@ -1625,19 +1712,19 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F33" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G33" t="s">
         <v>8</v>
@@ -1648,19 +1735,19 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F34" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
@@ -1671,19 +1758,19 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G35" t="s">
         <v>8</v>
@@ -1694,19 +1781,19 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
@@ -1717,19 +1804,19 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F37" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -1740,19 +1827,19 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F38" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G38" t="s">
         <v>8</v>
@@ -1763,19 +1850,19 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F39" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G39" t="s">
         <v>8</v>
@@ -1786,19 +1873,19 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G40" t="s">
         <v>8</v>
@@ -1809,19 +1896,19 @@
         <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F41" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G41" t="s">
         <v>8</v>
@@ -1832,19 +1919,19 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="F42" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="G42" t="s">
         <v>8</v>
@@ -1855,21 +1942,228 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E43" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
         <v>138</v>
       </c>
-      <c r="F43" t="s">
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" t="s">
+        <v>168</v>
+      </c>
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
         <v>139</v>
       </c>
-      <c r="G43" t="s">
+      <c r="D46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" t="s">
+        <v>168</v>
+      </c>
+      <c r="G46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" t="s">
+        <v>168</v>
+      </c>
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" t="s">
+        <v>165</v>
+      </c>
+      <c r="F50" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" t="s">
+        <v>154</v>
+      </c>
+      <c r="E51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" t="s">
+        <v>168</v>
+      </c>
+      <c r="G52" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1898,10 +2192,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -1913,7 +2207,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>

</xml_diff>